<commit_message>
WORK LOG FOR 11/15/2023
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\PCB design LLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74081BA3-BD0C-4A0B-8871-9A655C618A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48C3E15-D5E1-4E1F-BA32-3E00AD7BCF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="22">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>design</t>
+  </si>
+  <si>
+    <t>job interview</t>
+  </si>
+  <si>
+    <t>LED Ring schematic upload</t>
   </si>
 </sst>
 </file>
@@ -439,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +610,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>0.5</v>
       </c>
@@ -615,7 +621,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -626,7 +632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -637,7 +643,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -648,7 +654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
@@ -659,7 +665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -670,7 +676,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -681,7 +687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
@@ -692,7 +698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>0</v>
       </c>
@@ -702,8 +708,11 @@
       <c r="C25" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>1</v>
       </c>
@@ -714,77 +723,113 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>0.5</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>0</v>
       </c>
@@ -794,8 +839,11 @@
       <c r="C37" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>1</v>
       </c>
@@ -806,69 +854,82 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>0.5</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>11</v>
       </c>
@@ -880,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="2">
-        <v>45243</v>
+        <v>45250</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>4</v>
@@ -972,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="B61" s="2">
-        <v>45243</v>
+        <v>45251</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>4</v>
@@ -1064,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="2">
-        <v>45243</v>
+        <v>45252</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
work log 11/20/2023 + income and pay details
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\PCB design LLC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48C3E15-D5E1-4E1F-BA32-3E00AD7BCF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA2D498-ABF9-4119-A290-54874803446E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="27">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>LED Ring schematic upload</t>
+  </si>
+  <si>
+    <t>LED Ring Layout design</t>
+  </si>
+  <si>
+    <t>Pay</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>ZENBUSINESS $324.00</t>
+  </si>
+  <si>
+    <t>ZENBUSINESS $199.00</t>
   </si>
 </sst>
 </file>
@@ -114,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +148,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -146,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,6 +182,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -443,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,9 +479,12 @@
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -469,8 +497,17 @@
       <c r="D1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -480,57 +517,70 @@
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>0.45833333333333331</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>0.5</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -540,8 +590,9 @@
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -551,8 +602,9 @@
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -562,8 +614,9 @@
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
@@ -576,8 +629,14 @@
       <c r="D13">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
@@ -587,8 +646,14 @@
       <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>0.41666666666666669</v>
       </c>
@@ -598,8 +663,9 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>0.45833333333333331</v>
       </c>
@@ -609,8 +675,9 @@
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>0.5</v>
       </c>
@@ -620,8 +687,9 @@
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>5</v>
       </c>
@@ -631,8 +699,9 @@
       <c r="C18" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -642,8 +711,9 @@
       <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>7</v>
       </c>
@@ -653,8 +723,9 @@
       <c r="C20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
@@ -664,8 +735,9 @@
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -675,8 +747,9 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>10</v>
       </c>
@@ -686,8 +759,9 @@
       <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
@@ -697,8 +771,9 @@
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>0</v>
       </c>
@@ -711,8 +786,14 @@
       <c r="D25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>1</v>
       </c>
@@ -722,8 +803,14 @@
       <c r="C26" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>0.41666666666666669</v>
       </c>
@@ -733,8 +820,9 @@
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>0.45833333333333331</v>
       </c>
@@ -744,8 +832,9 @@
       <c r="C28" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>0.5</v>
       </c>
@@ -755,8 +844,9 @@
       <c r="C29" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
@@ -766,8 +856,9 @@
       <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
@@ -777,8 +868,9 @@
       <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -788,8 +880,9 @@
       <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>8</v>
       </c>
@@ -799,8 +892,9 @@
       <c r="C33" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
@@ -810,8 +904,9 @@
       <c r="C34" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>10</v>
       </c>
@@ -821,15 +916,17 @@
       <c r="C35" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>0</v>
       </c>
@@ -842,8 +939,14 @@
       <c r="D37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>1</v>
       </c>
@@ -853,8 +956,14 @@
       <c r="C38" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>0.41666666666666669</v>
       </c>
@@ -864,8 +973,9 @@
       <c r="C39" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>0.45833333333333331</v>
       </c>
@@ -875,8 +985,9 @@
       <c r="C40" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>0.5</v>
       </c>
@@ -886,57 +997,65 @@
       <c r="C41" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>0</v>
       </c>
@@ -946,8 +1065,17 @@
       <c r="C49" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>9</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>1</v>
       </c>
@@ -957,78 +1085,134 @@
       <c r="C50" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E50" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>0.5</v>
       </c>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>0</v>
       </c>
@@ -1038,8 +1222,14 @@
       <c r="C61" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E61" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>1</v>
       </c>
@@ -1049,78 +1239,94 @@
       <c r="C62" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E62" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>0.45833333333333331</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>0.5</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>0</v>
       </c>
@@ -1130,8 +1336,9 @@
       <c r="C73" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>1</v>
       </c>
@@ -1141,78 +1348,89 @@
       <c r="C74" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>0.45833333333333331</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>0.5</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E84" s="6"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>0</v>
       </c>
@@ -1222,8 +1440,9 @@
       <c r="C85" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>1</v>
       </c>
@@ -1233,76 +1452,183 @@
       <c r="C86" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E87" s="6"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>0.45833333333333331</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E88" s="6"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>0.5</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E90" s="6"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E91" s="6"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E92" s="6"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E93" s="6"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E94" s="6"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E95" s="6"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
+      <c r="E96" s="6"/>
+    </row>
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="6"/>
+    </row>
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E98" s="6"/>
+    </row>
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E99" s="6"/>
+    </row>
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E101" s="6"/>
+    </row>
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E102" s="6"/>
+    </row>
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E105" s="6"/>
+    </row>
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E106" s="6"/>
+    </row>
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E107" s="6"/>
+    </row>
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E108" s="6"/>
+    </row>
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E109" s="6"/>
+    </row>
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E110" s="6"/>
+    </row>
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E111" s="6"/>
+    </row>
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E112" s="6"/>
+    </row>
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E113" s="6"/>
+    </row>
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E114" s="6"/>
+    </row>
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E115" s="6"/>
+    </row>
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E116" s="6"/>
+    </row>
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E117" s="6"/>
+    </row>
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E118" s="6"/>
+    </row>
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E119" s="6"/>
+    </row>
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E121" s="6"/>
+    </row>
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E122" s="6"/>
+    </row>
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E123" s="6"/>
+    </row>
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E124" s="6"/>
+    </row>
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E125" s="6"/>
+    </row>
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E126" s="6"/>
+    </row>
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E127" s="6"/>
+    </row>
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E128" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
worklog update on 12/12/2023
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d134ffd41eb4789/PCB design LLC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B851D92-E069-4A1B-9225-E77ABDCA6DD3}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACDFB814-CFD5-4FA3-B31E-CC0C090B2FC9}"/>
   <bookViews>
     <workbookView xWindow="5235" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="30">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -218,6 +218,10 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -486,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="K182" sqref="K182"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,7 +2772,7 @@
         <v>4</v>
       </c>
       <c r="D181" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E181" s="7" t="s">
         <v>23</v>
@@ -2837,16 +2841,24 @@
       <c r="A186" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B186" s="1"/>
-      <c r="C186" s="1"/>
+      <c r="B186" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E186" s="6"/>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B187" s="1"/>
-      <c r="C187" s="1"/>
+      <c r="B187" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E187" s="6"/>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worklog update on 12/18/2023 and also use Clockify for worklog
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d134ffd41eb4789/PCB design LLC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACDFB814-CFD5-4FA3-B31E-CC0C090B2FC9}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63C8B46C-54BD-4AF3-9D07-DE3820C15419}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="450" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="37">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -115,6 +115,27 @@
   </si>
   <si>
     <t>Raspberry Pi 5V power schemetic design</t>
+  </si>
+  <si>
+    <t>NAS Python coding</t>
+  </si>
+  <si>
+    <t>NAS Python coding/UPLOAD</t>
+  </si>
+  <si>
+    <t>use another Worklog app Clockify</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>Math simulation on Python</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 5V power Layout design</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 5V power schemeticupload</t>
   </si>
 </sst>
 </file>
@@ -222,6 +243,14 @@
 </file>
 
 <file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -490,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="D181" sqref="D181"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="B222" sqref="B222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +837,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>23</v>
@@ -949,8 +978,12 @@
       <c r="A36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1485,8 +1518,12 @@
       <c r="A78" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E78" s="6"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -1742,10 +1779,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E99" s="6"/>
     </row>
@@ -1754,10 +1791,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E100" s="6"/>
     </row>
@@ -1766,10 +1803,10 @@
         <v>0.5</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E101" s="6"/>
     </row>
@@ -1778,10 +1815,10 @@
         <v>5</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E102" s="6"/>
     </row>
@@ -1790,10 +1827,10 @@
         <v>6</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E103" s="6"/>
     </row>
@@ -1937,8 +1974,12 @@
       <c r="A114" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
+      <c r="B114" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E114" s="6"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -2366,10 +2407,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E148" s="6"/>
     </row>
@@ -2378,10 +2419,10 @@
         <v>0.5</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E149" s="6"/>
     </row>
@@ -2389,8 +2430,12 @@
       <c r="A150" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
+      <c r="B150" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E150" s="6"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -2646,7 +2691,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>14</v>
@@ -2658,7 +2703,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>14</v>
@@ -2670,7 +2715,7 @@
         <v>0.5</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>14</v>
@@ -2682,7 +2727,7 @@
         <v>5</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>14</v>
@@ -2694,7 +2739,7 @@
         <v>6</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>14</v>
@@ -2706,7 +2751,7 @@
         <v>7</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>14</v>
@@ -2772,7 +2817,7 @@
         <v>4</v>
       </c>
       <c r="D181" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E181" s="7" t="s">
         <v>23</v>
@@ -2806,10 +2851,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E183" s="6"/>
     </row>
@@ -2818,10 +2863,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E184" s="6"/>
     </row>
@@ -2830,10 +2875,10 @@
         <v>0.5</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E185" s="6"/>
     </row>
@@ -2946,10 +2991,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E195" s="6"/>
     </row>
@@ -2958,10 +3003,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E196" s="6"/>
     </row>
@@ -2970,7 +3015,7 @@
         <v>0.5</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>19</v>
@@ -2982,10 +3027,10 @@
         <v>5</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E198" s="6"/>
     </row>
@@ -2994,7 +3039,7 @@
         <v>6</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>14</v>
@@ -3006,7 +3051,7 @@
         <v>7</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>14</v>
@@ -3018,10 +3063,10 @@
         <v>8</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E201" s="6"/>
     </row>
@@ -3030,7 +3075,7 @@
         <v>9</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>19</v>
@@ -3042,7 +3087,7 @@
         <v>10</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>19</v>
@@ -3054,7 +3099,7 @@
         <v>11</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>19</v>
@@ -3106,7 +3151,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>19</v>
@@ -3118,7 +3163,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>19</v>
@@ -3130,7 +3175,7 @@
         <v>0.5</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>19</v>
@@ -3142,7 +3187,7 @@
         <v>5</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>19</v>
@@ -3154,7 +3199,7 @@
         <v>6</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>19</v>
@@ -3166,7 +3211,7 @@
         <v>7</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>19</v>
@@ -3178,7 +3223,7 @@
         <v>8</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>19</v>
@@ -3190,7 +3235,7 @@
         <v>9</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>19</v>
@@ -3202,7 +3247,7 @@
         <v>10</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>19</v>
@@ -3214,7 +3259,7 @@
         <v>11</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>19</v>
@@ -3266,10 +3311,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E219" s="6"/>
     </row>
@@ -3278,10 +3323,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E220" s="6"/>
     </row>
@@ -3290,10 +3335,10 @@
         <v>0.5</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E221" s="6"/>
     </row>
@@ -3301,8 +3346,12 @@
       <c r="A222" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B222" s="1"/>
-      <c r="C222" s="1"/>
+      <c r="B222" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E222" s="6"/>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
worklog on 12/19/2023, sync on Clockify
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -251,6 +251,10 @@
 </file>
 
 <file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -519,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="B222" sqref="B222"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="B210" sqref="B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
worklog on 12/20/2023, sync on clockify
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -255,6 +255,10 @@
 </file>
 
 <file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -523,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="B210" sqref="B210"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="C219" sqref="C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
worklog update 12/27 /2023, sync on clockify
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d134ffd41eb4789/PCB design LLC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63C8B46C-54BD-4AF3-9D07-DE3820C15419}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7371260-FDD4-41A7-988E-B0548D935754}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="39">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Raspberry Pi 5V power schemeticupload</t>
+  </si>
+  <si>
+    <t>Machine learning digit recognition</t>
+  </si>
+  <si>
+    <t>find jobs</t>
   </si>
 </sst>
 </file>
@@ -259,6 +265,14 @@
 </file>
 
 <file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person6.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -525,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G228"/>
+  <dimension ref="A1:G264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="C219" sqref="C219"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C262" sqref="C262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3378,7 +3392,7 @@
       <c r="C224" s="1"/>
       <c r="E224" s="6"/>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>8</v>
       </c>
@@ -3386,7 +3400,7 @@
       <c r="C225" s="1"/>
       <c r="E225" s="6"/>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>9</v>
       </c>
@@ -3394,7 +3408,7 @@
       <c r="C226" s="1"/>
       <c r="E226" s="6"/>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>10</v>
       </c>
@@ -3402,13 +3416,473 @@
       <c r="C227" s="1"/>
       <c r="E227" s="6"/>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="E228" s="6"/>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B229" s="2">
+        <v>45287</v>
+      </c>
+      <c r="C229" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D229" s="8">
+        <v>9</v>
+      </c>
+      <c r="E229" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F229" t="s">
+        <v>25</v>
+      </c>
+      <c r="G229" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C230" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E230" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A231" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E231" s="6"/>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E232" s="6"/>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E233" s="6"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E234" s="6"/>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E235" s="6"/>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E236" s="6"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E237" s="6"/>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E238" s="6"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E239" s="6"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E240" s="6"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B241" s="2">
+        <v>45288</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D241" s="8">
+        <v>9</v>
+      </c>
+      <c r="E241" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F241" t="s">
+        <v>25</v>
+      </c>
+      <c r="G241" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E242" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E243" s="6"/>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E244" s="6"/>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E245" s="6"/>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E246" s="6"/>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E247" s="6"/>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E248" s="6"/>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E249" s="6"/>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E250" s="6"/>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E251" s="6"/>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E252" s="6"/>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B253" s="2">
+        <v>45289</v>
+      </c>
+      <c r="C253" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D253" s="8">
+        <v>4</v>
+      </c>
+      <c r="E253" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F253" t="s">
+        <v>25</v>
+      </c>
+      <c r="G253" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C254" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E254" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E255" s="6"/>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E256" s="6"/>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E257" s="6"/>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E258" s="6"/>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E259" s="6"/>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B260" s="1"/>
+      <c r="C260" s="1"/>
+      <c r="E260" s="6"/>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B261" s="1"/>
+      <c r="C261" s="1"/>
+      <c r="E261" s="6"/>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B262" s="1"/>
+      <c r="C262" s="1"/>
+      <c r="E262" s="6"/>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B263" s="1"/>
+      <c r="C263" s="1"/>
+      <c r="E263" s="6"/>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B264" s="1"/>
+      <c r="C264" s="1"/>
+      <c r="E264" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
worklog upload 12/28/2023 sync on clockify
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -276,6 +276,10 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person7.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -541,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C262" sqref="C262"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="D248" sqref="D248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
WORKLOG SYNC, SAME ON CLOCKIFY
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d134ffd41eb4789/PCB design LLC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7371260-FDD4-41A7-988E-B0548D935754}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{394320DD-854C-421D-9C77-62462A1F7564}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="39">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -277,6 +277,10 @@
 </file>
 
 <file path=xl/persons/person7.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person8.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -543,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G264"/>
+  <dimension ref="A1:G372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="D248" sqref="D248"/>
+    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
+      <selection activeCell="J351" sqref="J351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,7 +3816,7 @@
       </c>
       <c r="E256" s="6"/>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>0.5</v>
       </c>
@@ -3824,7 +3828,7 @@
       </c>
       <c r="E257" s="6"/>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
         <v>5</v>
       </c>
@@ -3836,7 +3840,7 @@
       </c>
       <c r="E258" s="6"/>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
         <v>6</v>
       </c>
@@ -3848,7 +3852,7 @@
       </c>
       <c r="E259" s="6"/>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="3" t="s">
         <v>7</v>
       </c>
@@ -3856,7 +3860,7 @@
       <c r="C260" s="1"/>
       <c r="E260" s="6"/>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
         <v>8</v>
       </c>
@@ -3864,7 +3868,7 @@
       <c r="C261" s="1"/>
       <c r="E261" s="6"/>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
         <v>9</v>
       </c>
@@ -3872,7 +3876,7 @@
       <c r="C262" s="1"/>
       <c r="E262" s="6"/>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="3" t="s">
         <v>10</v>
       </c>
@@ -3880,13 +3884,1393 @@
       <c r="C263" s="1"/>
       <c r="E263" s="6"/>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B264" s="1"/>
       <c r="C264" s="1"/>
       <c r="E264" s="6"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B265" s="2">
+        <v>45293</v>
+      </c>
+      <c r="C265" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D265" s="8">
+        <v>9</v>
+      </c>
+      <c r="E265" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F265" t="s">
+        <v>25</v>
+      </c>
+      <c r="G265" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E266" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E267" s="6"/>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E268" s="6"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E269" s="6"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E270" s="6"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E271" s="6"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E272" s="6"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E273" s="6"/>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E274" s="6"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E275" s="6"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E276" s="6"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B277" s="2">
+        <v>45294</v>
+      </c>
+      <c r="C277" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D277" s="8">
+        <v>9</v>
+      </c>
+      <c r="E277" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F277" t="s">
+        <v>25</v>
+      </c>
+      <c r="G277" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C278" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E278" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E279" s="6"/>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E280" s="6"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E281" s="6"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E282" s="6"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E283" s="6"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E284" s="6"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E285" s="6"/>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E286" s="6"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E287" s="6"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E288" s="6"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B289" s="2">
+        <v>45295</v>
+      </c>
+      <c r="C289" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D289" s="8">
+        <v>4</v>
+      </c>
+      <c r="E289" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F289" t="s">
+        <v>25</v>
+      </c>
+      <c r="G289" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C290" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E290" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E291" s="6"/>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E292" s="6"/>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E293" s="6"/>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E294" s="6"/>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E295" s="6"/>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B296" s="1"/>
+      <c r="C296" s="1"/>
+      <c r="E296" s="6"/>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B297" s="1"/>
+      <c r="C297" s="1"/>
+      <c r="E297" s="6"/>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B298" s="1"/>
+      <c r="C298" s="1"/>
+      <c r="E298" s="6"/>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B299" s="1"/>
+      <c r="C299" s="1"/>
+      <c r="E299" s="6"/>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B300" s="1"/>
+      <c r="C300" s="1"/>
+      <c r="E300" s="6"/>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B301" s="2">
+        <v>45299</v>
+      </c>
+      <c r="C301" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D301" s="8">
+        <v>9</v>
+      </c>
+      <c r="E301" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F301" t="s">
+        <v>25</v>
+      </c>
+      <c r="G301" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C302" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E302" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F302">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E303" s="6"/>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E304" s="6"/>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E305" s="6"/>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E306" s="6"/>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E307" s="6"/>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E308" s="6"/>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E309" s="6"/>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E310" s="6"/>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E311" s="6"/>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E312" s="6"/>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B313" s="2">
+        <v>45300</v>
+      </c>
+      <c r="C313" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D313" s="8">
+        <v>9</v>
+      </c>
+      <c r="E313" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F313" t="s">
+        <v>25</v>
+      </c>
+      <c r="G313" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B314" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C314" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E314" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E315" s="6"/>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E316" s="6"/>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E317" s="6"/>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E318" s="6"/>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E319" s="6"/>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A320" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E320" s="6"/>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A321" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E321" s="6"/>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A322" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E322" s="6"/>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A323" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E323" s="6"/>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A324" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E324" s="6"/>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A325" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B325" s="2">
+        <v>45301</v>
+      </c>
+      <c r="C325" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D325" s="8">
+        <v>4</v>
+      </c>
+      <c r="E325" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F325" t="s">
+        <v>25</v>
+      </c>
+      <c r="G325" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A326" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B326" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C326" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E326" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A327" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E327" s="6"/>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A328" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E328" s="6"/>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A329" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E329" s="6"/>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A330" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E330" s="6"/>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A331" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E331" s="6"/>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A332" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B332" s="1"/>
+      <c r="C332" s="1"/>
+      <c r="E332" s="6"/>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A333" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B333" s="1"/>
+      <c r="C333" s="1"/>
+      <c r="E333" s="6"/>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A334" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B334" s="1"/>
+      <c r="C334" s="1"/>
+      <c r="E334" s="6"/>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A335" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B335" s="1"/>
+      <c r="C335" s="1"/>
+      <c r="E335" s="6"/>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A336" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B336" s="1"/>
+      <c r="C336" s="1"/>
+      <c r="E336" s="6"/>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A337" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B337" s="2">
+        <v>45307</v>
+      </c>
+      <c r="C337" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D337" s="8">
+        <v>9</v>
+      </c>
+      <c r="E337" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F337" t="s">
+        <v>25</v>
+      </c>
+      <c r="G337" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A338" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B338" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C338" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E338" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F338">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A339" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E339" s="6"/>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A340" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E340" s="6"/>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A341" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E341" s="6"/>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A342" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E342" s="6"/>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A343" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E343" s="6"/>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A344" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E344" s="6"/>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A345" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E345" s="6"/>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A346" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E346" s="6"/>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A347" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E347" s="6"/>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A348" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E348" s="6"/>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A349" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B349" s="2">
+        <v>45308</v>
+      </c>
+      <c r="C349" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D349" s="8">
+        <v>9</v>
+      </c>
+      <c r="E349" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F349" t="s">
+        <v>25</v>
+      </c>
+      <c r="G349" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A350" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B350" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C350" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E350" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A351" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E351" s="6"/>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A352" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E352" s="6"/>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A353" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E353" s="6"/>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A354" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E354" s="6"/>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A355" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E355" s="6"/>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A356" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E356" s="6"/>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A357" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E357" s="6"/>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A358" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E358" s="6"/>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A359" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E359" s="6"/>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A360" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E360" s="6"/>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A361" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B361" s="2">
+        <v>45309</v>
+      </c>
+      <c r="C361" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D361" s="8">
+        <v>4</v>
+      </c>
+      <c r="E361" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F361" t="s">
+        <v>25</v>
+      </c>
+      <c r="G361" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A362" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B362" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C362" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E362" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A363" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E363" s="6"/>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A364" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E364" s="6"/>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A365" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E365" s="6"/>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A366" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E366" s="6"/>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A367" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E367" s="6"/>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A368" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B368" s="1"/>
+      <c r="C368" s="1"/>
+      <c r="E368" s="6"/>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A369" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B369" s="1"/>
+      <c r="C369" s="1"/>
+      <c r="E369" s="6"/>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A370" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B370" s="1"/>
+      <c r="C370" s="1"/>
+      <c r="E370" s="6"/>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A371" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B371" s="1"/>
+      <c r="C371" s="1"/>
+      <c r="E371" s="6"/>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A372" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B372" s="1"/>
+      <c r="C372" s="1"/>
+      <c r="E372" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
worklog update 1/4/2024 sync on clockify
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d134ffd41eb4789/PCB design LLC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{394320DD-854C-421D-9C77-62462A1F7564}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00CDB221-EFA5-4BF2-9044-A42ECF66E17D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="40">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>find jobs</t>
+  </si>
+  <si>
+    <t>Worked on surface profiling paper</t>
   </si>
 </sst>
 </file>
@@ -281,6 +284,10 @@
 </file>
 
 <file path=xl/persons/person8.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person9.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -549,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
-      <selection activeCell="J351" sqref="J351"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="C295" sqref="C295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4257,10 +4264,10 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E291" s="6"/>
     </row>
@@ -4269,10 +4276,10 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E292" s="6"/>
     </row>
@@ -4281,10 +4288,10 @@
         <v>0.5</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E293" s="6"/>
     </row>
@@ -4293,10 +4300,10 @@
         <v>5</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E294" s="6"/>
     </row>
@@ -4305,10 +4312,10 @@
         <v>6</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E295" s="6"/>
     </row>

</xml_diff>

<commit_message>
worklog update on 1/8/2024 sync on clockify
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d134ffd41eb4789/PCB design LLC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00CDB221-EFA5-4BF2-9044-A42ECF66E17D}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEA6CB1E-3642-485C-B986-572D21F13197}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="41">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -146,6 +146,9 @@
   <si>
     <t>Worked on surface profiling paper</t>
   </si>
+  <si>
+    <t>job process</t>
+  </si>
 </sst>
 </file>
 
@@ -256,6 +259,10 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person10.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -556,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="C295" sqref="C295"/>
+    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
+      <selection activeCell="B330" sqref="B330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4600,7 +4607,7 @@
         <v>5</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>14</v>
@@ -4612,7 +4619,7 @@
         <v>6</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C319" s="1" t="s">
         <v>14</v>
@@ -4624,7 +4631,7 @@
         <v>7</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C320" s="1" t="s">
         <v>14</v>
@@ -4636,7 +4643,7 @@
         <v>8</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C321" s="1" t="s">
         <v>14</v>
@@ -4648,7 +4655,7 @@
         <v>9</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C322" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
worklog on 1/16/2024 sync on clockify
</commit_message>
<xml_diff>
--- a/Company Work Log.xlsx
+++ b/Company Work Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d134ffd41eb4789/PCB design LLC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEA6CB1E-3642-485C-B986-572D21F13197}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{3CEB2D3C-4C3D-4009-A667-693E91A4E3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76D96196-17B2-4FAD-901E-7E2A68912E95}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="43">
   <si>
     <t xml:space="preserve"> Date</t>
   </si>
@@ -149,6 +149,12 @@
   <si>
     <t>job process</t>
   </si>
+  <si>
+    <t>job discussion</t>
+  </si>
+  <si>
+    <t>bussiness close preperation</t>
+  </si>
 </sst>
 </file>
 
@@ -248,54 +254,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person10.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person6.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person7.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person8.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person9.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -563,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
-      <selection activeCell="B330" sqref="B330"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="C370" sqref="C370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4919,10 +4877,10 @@
         <v>6</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E343" s="6"/>
     </row>
@@ -4931,10 +4889,10 @@
         <v>7</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E344" s="6"/>
     </row>
@@ -4943,10 +4901,10 @@
         <v>8</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E345" s="6"/>
     </row>
@@ -4955,10 +4913,10 @@
         <v>9</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E346" s="6"/>
     </row>
@@ -4967,10 +4925,10 @@
         <v>10</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E347" s="6"/>
     </row>
@@ -4979,10 +4937,10 @@
         <v>11</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E348" s="6"/>
     </row>
@@ -5067,10 +5025,10 @@
         <v>5</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E354" s="6"/>
     </row>
@@ -5079,10 +5037,10 @@
         <v>6</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E355" s="6"/>
     </row>
@@ -5091,10 +5049,10 @@
         <v>7</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E356" s="6"/>
     </row>
@@ -5103,10 +5061,10 @@
         <v>8</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E357" s="6"/>
     </row>
@@ -5115,7 +5073,7 @@
         <v>9</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>14</v>
@@ -5127,10 +5085,10 @@
         <v>10</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E359" s="6"/>
     </row>
@@ -5139,10 +5097,10 @@
         <v>11</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E360" s="6"/>
     </row>
@@ -5227,10 +5185,10 @@
         <v>5</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E366" s="6"/>
     </row>
@@ -5239,10 +5197,10 @@
         <v>6</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E367" s="6"/>
     </row>

</xml_diff>